<commit_message>
Updates to the menu to allow sub-menus
</commit_message>
<xml_diff>
--- a/DevTools.xlsx
+++ b/DevTools.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/256c97ba8ed48425/Documents/Projects/PBX/RasPBX_Build/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="13_ncr:1_{1C4A9213-C812-4D7A-B2C0-60F82FA4474B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD763C9F-35A4-453B-8747-A5F5DA8FA449}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{1C4A9213-C812-4D7A-B2C0-60F82FA4474B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62534B86-2E0A-4753-8C6A-915BAD29FE78}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="3" xr2:uid="{0A6266C4-26DD-4DE6-B06A-1B7D997BFB8E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{0A6266C4-26DD-4DE6-B06A-1B7D997BFB8E}"/>
   </bookViews>
   <sheets>
     <sheet name="jomisEnvironments" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="292">
   <si>
     <t>URL to Landing Page</t>
   </si>
@@ -673,9 +673,6 @@
     <t>MHS G-T Information Request</t>
   </si>
   <si>
-    <t>host_url</t>
-  </si>
-  <si>
     <t>~/js/modal.js</t>
   </si>
   <si>
@@ -760,9 +757,6 @@
     <t>installation_update</t>
   </si>
   <si>
-    <t>local_url</t>
-  </si>
-  <si>
     <t>1. Install RasPBX</t>
   </si>
   <si>
@@ -808,9 +802,6 @@
     <t>Linphone (Softphone)</t>
   </si>
   <si>
-    <t>Cisco 79xx IP Phones</t>
-  </si>
-  <si>
     <t>phones_linphone</t>
   </si>
   <si>
@@ -893,6 +884,48 @@
   </si>
   <si>
     <t>~/about/references.html</t>
+  </si>
+  <si>
+    <t>menu_js</t>
+  </si>
+  <si>
+    <t>~/js/menu.js</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>phones_cisco79xx_reset</t>
+  </si>
+  <si>
+    <t>phones_cisco79xx_tftp</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Setup TFTP</t>
+  </si>
+  <si>
+    <t>XML Config</t>
+  </si>
+  <si>
+    <t>phones_cisco79xx_xml</t>
+  </si>
+  <si>
+    <t>phones_cisco79xx_directory</t>
+  </si>
+  <si>
+    <t>Directory</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>phones_cisco79xx_services</t>
   </si>
 </sst>
 </file>
@@ -2399,10 +2432,10 @@
   <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,16 +2457,16 @@
         <v>108</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>236</v>
+        <v>280</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>207</v>
+        <v>281</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>24</v>
       </c>
@@ -2443,18 +2476,20 @@
       <c r="C2" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="E2" s="12" t="s">
         <v>27</v>
       </c>
       <c r="F2" s="10" t="str">
         <f>IF(A2="","","    { " &amp; $A$1 &amp; ": """ &amp; A2 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B2 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C2) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D2 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E2 &amp; """}" &amp; IF(A3="","",","))</f>
-        <v xml:space="preserve">    { id: "jquery_slim_min_js", fileType: "script", req_jquery: false, local_url: "", host_url: "https://code.jquery.com/jquery-3.5.1.slim.min.js"},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "jquery_slim_min_js", fileType: "script", req_jquery: false, local: "https://code.jquery.com/jquery-3.5.1.slim.min.js", host: "https://code.jquery.com/jquery-3.5.1.slim.min.js"},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>26</v>
@@ -2462,18 +2497,20 @@
       <c r="C3" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>218</v>
+      </c>
       <c r="E3" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F3" s="10" t="str">
         <f t="shared" ref="F3:F15" si="0">IF(A3="","","    { " &amp; $A$1 &amp; ": """ &amp; A3 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B3 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C3) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D3 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E3 &amp; """}" &amp; IF(A4="","",","))</f>
-        <v xml:space="preserve">    { id: "jquery_min_js", fileType: "script", req_jquery: false, local_url: "", host_url: "https://code.jquery.com/jquery-3.5.1.min.js"},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "jquery_min_js", fileType: "script", req_jquery: false, local: "https://code.jquery.com/jquery-3.5.1.min.js", host: "https://code.jquery.com/jquery-3.5.1.min.js"},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>26</v>
@@ -2481,18 +2518,20 @@
       <c r="C4" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>220</v>
+      </c>
       <c r="E4" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F4" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_content", fileType: "script", req_jquery: false, local_url: "", host_url: "~/js/content.js"},</v>
+        <v xml:space="preserve">    { id: "js_content", fileType: "script", req_jquery: false, local: "~/js/content.js", host: "~/js/content.js"},</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>26</v>
@@ -2500,18 +2539,20 @@
       <c r="C5" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>207</v>
+      </c>
       <c r="E5" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F5" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_modal", fileType: "script", req_jquery: false, local_url: "", host_url: "~/js/modal.js"},</v>
+        <v xml:space="preserve">    { id: "js_modal", fileType: "script", req_jquery: false, local: "~/js/modal.js", host: "~/js/modal.js"},</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>26</v>
@@ -2519,18 +2560,20 @@
       <c r="C6" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>223</v>
+      </c>
       <c r="E6" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F6" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_header", fileType: "script", req_jquery: false, local_url: "", host_url: "~/js/header.js"},</v>
+        <v xml:space="preserve">    { id: "js_header", fileType: "script", req_jquery: false, local: "~/js/header.js", host: "~/js/header.js"},</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>26</v>
@@ -2538,18 +2581,20 @@
       <c r="C7" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>224</v>
+      </c>
       <c r="E7" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F7" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_footer", fileType: "script", req_jquery: false, local_url: "", host_url: "~/js/footer.js"},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "js_footer", fileType: "script", req_jquery: false, local: "~/js/footer.js", host: "~/js/footer.js"},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>29</v>
@@ -2557,18 +2602,20 @@
       <c r="C8" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>208</v>
+      </c>
       <c r="E8" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F8" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_main", fileType: "style", req_jquery: false, local_url: "", host_url: "~/style/main.css"},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "js_main", fileType: "style", req_jquery: false, local: "~/style/main.css", host: "~/style/main.css"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>29</v>
@@ -2576,18 +2623,20 @@
       <c r="C9" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>209</v>
+      </c>
       <c r="E9" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_modal", fileType: "style", req_jquery: false, local_url: "", host_url: "~/style/modal.css"},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_modal", fileType: "style", req_jquery: false, local: "~/style/modal.css", host: "~/style/modal.css"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>29</v>
@@ -2595,18 +2644,20 @@
       <c r="C10" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>210</v>
+      </c>
       <c r="E10" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_imagebox", fileType: "style", req_jquery: false, local_url: "", host_url: "~/style/imageBox.css"},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_imagebox", fileType: "style", req_jquery: false, local: "~/style/imageBox.css", host: "~/style/imageBox.css"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>29</v>
@@ -2614,18 +2665,20 @@
       <c r="C11" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="10"/>
+      <c r="D11" s="10" t="s">
+        <v>211</v>
+      </c>
       <c r="E11" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_imgtitle", fileType: "style", req_jquery: false, local_url: "", host_url: "~/style/imgtitle.css"},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_imgtitle", fileType: "style", req_jquery: false, local: "~/style/imgtitle.css", host: "~/style/imgtitle.css"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>29</v>
@@ -2633,18 +2686,20 @@
       <c r="C12" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>227</v>
+      </c>
       <c r="E12" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_menu", fileType: "style", req_jquery: false, local_url: "", host_url: "~/style/menu.css"},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_menu", fileType: "style", req_jquery: false, local: "~/style/menu.css", host: "~/style/menu.css"},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>29</v>
@@ -2652,16 +2707,18 @@
       <c r="C13" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>228</v>
+      </c>
       <c r="E13" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_default", fileType: "style", req_jquery: false, local_url: "", host_url: "~/style/default.css"},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_default", fileType: "style", req_jquery: false, local: "~/style/default.css", host: "~/style/default.css"},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>28</v>
       </c>
@@ -2671,13 +2728,15 @@
       <c r="C14" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="E14" s="10" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "bootstrap_min_css", fileType: "style", req_jquery: true, local_url: "", host_url: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css"},</v>
+        <v xml:space="preserve">    { id: "bootstrap_min_css", fileType: "style", req_jquery: true, local: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css", host: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css"},</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2690,24 +2749,36 @@
       <c r="C15" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="10" t="s">
         <v>32</v>
       </c>
       <c r="F15" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "bootstrap_bundle_min_js", fileType: "script", req_jquery: true, local_url: "", host_url: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.bundle.min.js"}</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
+        <v xml:space="preserve">    { id: "bootstrap_bundle_min_js", fileType: "script", req_jquery: true, local: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.bundle.min.js", host: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.bundle.min.js"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="F16" s="10" t="str">
         <f t="shared" ref="F16:F72" si="1">IF(A16="","","    { " &amp; $A$1 &amp; ": """ &amp; A16 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B16 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C16) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D16 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E16 &amp; """}" &amp; IF(A17="","",","))</f>
-        <v/>
+        <v xml:space="preserve">    { id: "menu_js", fileType: "script", req_jquery: true, local: "~/js/menu.js", host: "~/js/menu.js"}</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3710,21 +3781,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D934C6D7-8A74-4B09-A541-AF970631420F}">
   <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F2:F12"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F2:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="82" style="4" customWidth="1"/>
+    <col min="6" max="6" width="125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3754,7 +3825,7 @@
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="10" t="str">
@@ -3764,16 +3835,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="10" t="str">
@@ -3783,16 +3854,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10" t="str">
@@ -3802,16 +3873,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="str">
@@ -3821,16 +3892,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="10" t="str">
@@ -3840,16 +3911,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="D7" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>248</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10" t="str">
@@ -3859,16 +3930,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>246</v>
-      </c>
       <c r="C8" s="9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="str">
@@ -3878,16 +3949,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10" t="str">
@@ -3897,16 +3968,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10" t="str">
@@ -3916,84 +3987,116 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>254</v>
+        <v>282</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "phones_cisco79xx", group: "Phones", name: "Cisco 79xx IP Phones", url: "~/phones/cisco79xx.html", target: ""},</v>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_reset", group: "Phones", name: "Reset", url: "~/phones/cisco79xx.html", target: ""},</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>74</v>
+        <v>248</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "about_references", group: "About", name: "References", url: "~/about/references.html", target: ""}</v>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_tftp", group: "Phones", name: "Setup TFTP", url: "~/phones/cisco79xx.html", target: ""},</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>259</v>
+      </c>
       <c r="E13" s="9"/>
       <c r="F13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_xml", group: "Phones", name: "XML Config", url: "~/phones/cisco79xx.html", target: ""},</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>259</v>
+      </c>
       <c r="E14" s="9"/>
       <c r="F14" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_directory", group: "Phones", name: "Directory", url: "~/phones/cisco79xx.html", target: ""},</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="A15" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>259</v>
+      </c>
       <c r="E15" s="9"/>
       <c r="F15" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_services", group: "Phones", name: "Services", url: "~/phones/cisco79xx.html", target: ""},</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="A16" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>277</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="10" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">    { id: "about_references", group: "About", name: "References", url: "~/about/references.html", target: ""}</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4996,7 +5099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D83757-FC48-42CC-A84E-A75FA6AFBAAD}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5020,10 +5123,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>20</v>
@@ -5031,13 +5134,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D2" s="9" t="str">
         <f>IF(B2="","",B2) &amp; IF(C2="","",C2 &amp; "/")</f>
@@ -5050,13 +5153,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D3" s="9" t="str">
         <f t="shared" ref="D3:D10" si="0">IF(B3="","",B3) &amp; IF(C3="","",C3 &amp; "/")</f>
@@ -5069,13 +5172,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D4" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5088,13 +5191,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D5" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5107,13 +5210,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D6" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5126,13 +5229,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D7" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5145,13 +5248,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D8" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5164,13 +5267,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>275</v>
       </c>
       <c r="D9" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5183,13 +5286,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D10" s="9" t="str">
         <f t="shared" si="0"/>
@@ -5202,13 +5305,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D11" s="9" t="str">
         <f>IF(B11="","",B11) &amp; IF(C11="","",C11 &amp; "/")</f>

</xml_diff>

<commit_message>
- Added separate pages for configuring Cisco 79xx phones - Added status PowerPoint slide
</commit_message>
<xml_diff>
--- a/DevTools.xlsx
+++ b/DevTools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/256c97ba8ed48425/Documents/Projects/PBX/RasPBX_Build/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{1C4A9213-C812-4D7A-B2C0-60F82FA4474B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62534B86-2E0A-4753-8C6A-915BAD29FE78}"/>
+  <xr:revisionPtr revIDLastSave="454" documentId="13_ncr:1_{1C4A9213-C812-4D7A-B2C0-60F82FA4474B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11F528B0-6F11-4568-B797-34DE7F0F4E41}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{0A6266C4-26DD-4DE6-B06A-1B7D997BFB8E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="324">
   <si>
     <t>URL to Landing Page</t>
   </si>
@@ -829,9 +829,6 @@
     <t>phones/</t>
   </si>
   <si>
-    <t>~/phones/cisco79xx.html</t>
-  </si>
-  <si>
     <t>installation</t>
   </si>
   <si>
@@ -886,9 +883,6 @@
     <t>~/about/references.html</t>
   </si>
   <si>
-    <t>menu_js</t>
-  </si>
-  <si>
     <t>~/js/menu.js</t>
   </si>
   <si>
@@ -926,6 +920,108 @@
   </si>
   <si>
     <t>phones_cisco79xx_services</t>
+  </si>
+  <si>
+    <t>test_header</t>
+  </si>
+  <si>
+    <t>test_footer</t>
+  </si>
+  <si>
+    <t>js/</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>font_awesome</t>
+  </si>
+  <si>
+    <t>mdbootstrap_footer</t>
+  </si>
+  <si>
+    <t>sample_mdbootstrap_footer</t>
+  </si>
+  <si>
+    <t>https://kit.fontawesome.com/a12f3f2147.js</t>
+  </si>
+  <si>
+    <t>style_main</t>
+  </si>
+  <si>
+    <t>~/js/main.js</t>
+  </si>
+  <si>
+    <t>js_menu</t>
+  </si>
+  <si>
+    <t>Cisco79xx</t>
+  </si>
+  <si>
+    <t>~/phones/cisco79xx_reset.html</t>
+  </si>
+  <si>
+    <t>~/phones/cisco79xx_tftp.html</t>
+  </si>
+  <si>
+    <t>~/phones/cisco79xx_xml.html</t>
+  </si>
+  <si>
+    <t>~/phones/cisco79xx_directory.html</t>
+  </si>
+  <si>
+    <t>~/phones/cisco79xx_services.html</t>
+  </si>
+  <si>
+    <t>Cisco 79xx</t>
+  </si>
+  <si>
+    <t>remote_mariadb</t>
+  </si>
+  <si>
+    <t>MariaDB</t>
+  </si>
+  <si>
+    <t>~/remote/mariadb.html</t>
+  </si>
+  <si>
+    <t>mariadb</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Does not require jQuery but needs to load last</t>
+  </si>
+  <si>
+    <t>More</t>
+  </si>
+  <si>
+    <t>Cisco 79xx Misc. Info</t>
+  </si>
+  <si>
+    <t>~/more/cisco79xx_misc.html</t>
+  </si>
+  <si>
+    <t>more_cisco79xx_misc</t>
+  </si>
+  <si>
+    <t>more/</t>
+  </si>
+  <si>
+    <t>cisco79xx_misc</t>
+  </si>
+  <si>
+    <t>phones_cisco79xx_extension</t>
+  </si>
+  <si>
+    <t>~/phones/cisco79xx_extension.html</t>
+  </si>
+  <si>
+    <t>Add Extension(s)</t>
   </si>
 </sst>
 </file>
@@ -964,12 +1060,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1000,7 +1102,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1028,6 +1130,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2429,24 +2536,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0133D875-A617-42E7-858D-1BB6ED82B6FF}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F15:F16"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="50.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="50.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>23</v>
       </c>
@@ -2457,18 +2565,21 @@
         <v>108</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>24</v>
+        <v>295</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>26</v>
@@ -2476,20 +2587,21 @@
       <c r="C2" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>27</v>
+      <c r="D2" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>298</v>
       </c>
       <c r="F2" s="10" t="str">
         <f>IF(A2="","","    { " &amp; $A$1 &amp; ": """ &amp; A2 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B2 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C2) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D2 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E2 &amp; """}" &amp; IF(A3="","",","))</f>
-        <v xml:space="preserve">    { id: "jquery_slim_min_js", fileType: "script", req_jquery: false, local: "https://code.jquery.com/jquery-3.5.1.slim.min.js", host: "https://code.jquery.com/jquery-3.5.1.slim.min.js"},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "font_awesome", fileType: "script", req_jquery: false, local: "https://kit.fontawesome.com/a12f3f2147.js", host: "https://kit.fontawesome.com/a12f3f2147.js"},</v>
+      </c>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>26</v>
@@ -2497,20 +2609,21 @@
       <c r="C3" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>218</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>218</v>
+      <c r="D3" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>300</v>
       </c>
       <c r="F3" s="10" t="str">
         <f t="shared" ref="F3:F15" si="0">IF(A3="","","    { " &amp; $A$1 &amp; ": """ &amp; A3 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B3 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C3) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D3 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E3 &amp; """}" &amp; IF(A4="","",","))</f>
-        <v xml:space="preserve">    { id: "jquery_min_js", fileType: "script", req_jquery: false, local: "https://code.jquery.com/jquery-3.5.1.min.js", host: "https://code.jquery.com/jquery-3.5.1.min.js"},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "js_main", fileType: "script", req_jquery: false, local: "~/js/main.js", host: "~/js/main.js"},</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>26</v>
@@ -2519,19 +2632,20 @@
         <v>0</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="F4" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_content", fileType: "script", req_jquery: false, local: "~/js/content.js", host: "~/js/content.js"},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "js_modal", fileType: "script", req_jquery: false, local: "~/js/modal.js", host: "~/js/modal.js"},</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>216</v>
+        <v>24</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>26</v>
@@ -2539,20 +2653,21 @@
       <c r="C5" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>207</v>
+      <c r="D5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="F5" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_modal", fileType: "script", req_jquery: false, local: "~/js/modal.js", host: "~/js/modal.js"},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "jquery_slim_min_js", fileType: "script", req_jquery: false, local: "https://code.jquery.com/jquery-3.5.1.slim.min.js", host: "https://code.jquery.com/jquery-3.5.1.slim.min.js"},</v>
+      </c>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>26</v>
@@ -2560,20 +2675,21 @@
       <c r="C6" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>223</v>
+      <c r="D6" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="F6" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_header", fileType: "script", req_jquery: false, local: "~/js/header.js", host: "~/js/header.js"},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "jquery_min_js", fileType: "script", req_jquery: false, local: "https://code.jquery.com/jquery-3.5.1.min.js", host: "https://code.jquery.com/jquery-3.5.1.min.js"},</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>26</v>
@@ -2582,61 +2698,68 @@
         <v>0</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "js_content", fileType: "script", req_jquery: false, local: "~/js/content.js", host: "~/js/content.js"},</v>
+      </c>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="F8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "js_header", fileType: "script", req_jquery: true, local: "~/js/header.js", host: "~/js/header.js"},</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="F7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_footer", fileType: "script", req_jquery: false, local: "~/js/footer.js", host: "~/js/footer.js"},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="F8" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "js_main", fileType: "style", req_jquery: false, local: "~/style/main.css", host: "~/style/main.css"},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>209</v>
-      </c>
       <c r="F9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_modal", fileType: "style", req_jquery: false, local: "~/style/modal.css", host: "~/style/modal.css"},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "js_footer", fileType: "script", req_jquery: true, local: "~/js/footer.js", host: "~/js/footer.js"},</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>213</v>
+        <v>299</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>29</v>
@@ -2645,19 +2768,20 @@
         <v>0</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_imagebox", fileType: "style", req_jquery: false, local: "~/style/imageBox.css", host: "~/style/imageBox.css"},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_main", fileType: "style", req_jquery: false, local: "~/style/main.css", host: "~/style/main.css"},</v>
+      </c>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>29</v>
@@ -2666,19 +2790,20 @@
         <v>0</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_imgtitle", fileType: "style", req_jquery: false, local: "~/style/imgtitle.css", host: "~/style/imgtitle.css"},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_modal", fileType: "style", req_jquery: false, local: "~/style/modal.css", host: "~/style/modal.css"},</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>29</v>
@@ -2687,19 +2812,20 @@
         <v>0</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_menu", fileType: "style", req_jquery: false, local: "~/style/menu.css", host: "~/style/menu.css"},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_imagebox", fileType: "style", req_jquery: false, local: "~/style/imageBox.css", host: "~/style/imageBox.css"},</v>
+      </c>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>29</v>
@@ -2708,102 +2834,128 @@
         <v>0</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="F13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "style_default", fileType: "style", req_jquery: false, local: "~/style/default.css", host: "~/style/default.css"},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_imgtitle", fileType: "style", req_jquery: false, local: "~/style/imgtitle.css", host: "~/style/imgtitle.css"},</v>
+      </c>
+      <c r="G13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>28</v>
+        <v>225</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>31</v>
+        <v>227</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>31</v>
+        <v>227</v>
       </c>
       <c r="F14" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "bootstrap_min_css", fileType: "style", req_jquery: true, local: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css", host: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css"},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_menu", fileType: "style", req_jquery: false, local: "~/style/menu.css", host: "~/style/menu.css"},</v>
+      </c>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>30</v>
+        <v>226</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C15" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>32</v>
+        <v>228</v>
       </c>
       <c r="F15" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "bootstrap_bundle_min_js", fileType: "script", req_jquery: true, local: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.bundle.min.js", host: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.bundle.min.js"},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "style_default", fileType: "style", req_jquery: false, local: "~/style/default.css", host: "~/style/default.css"},</v>
+      </c>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>278</v>
+        <v>28</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" s="9" t="b">
         <v>1</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>279</v>
+        <v>31</v>
       </c>
       <c r="F16" s="10" t="str">
         <f t="shared" ref="F16:F72" si="1">IF(A16="","","    { " &amp; $A$1 &amp; ": """ &amp; A16 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B16 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C16) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D16 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E16 &amp; """}" &amp; IF(A17="","",","))</f>
-        <v xml:space="preserve">    { id: "menu_js", fileType: "script", req_jquery: true, local: "~/js/menu.js", host: "~/js/menu.js"}</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+        <v xml:space="preserve">    { id: "bootstrap_min_css", fileType: "style", req_jquery: true, local: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css", host: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css"},</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="F17" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+        <v xml:space="preserve">    { id: "bootstrap_bundle_min_js", fileType: "script", req_jquery: true, local: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.bundle.min.js", host: "https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.bundle.min.js"},</v>
+      </c>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="F18" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { id: "js_menu", fileType: "script", req_jquery: true, local: "~/js/menu.js", host: "~/js/menu.js"}</v>
+      </c>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -2813,8 +2965,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -2824,8 +2977,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -2835,8 +2989,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2846,8 +3001,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2857,8 +3013,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -2868,8 +3025,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2879,8 +3037,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -2890,8 +3049,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -2901,8 +3061,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -2912,8 +3073,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -2923,8 +3085,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -2934,8 +3097,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -2945,8 +3109,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -2956,8 +3121,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -2967,8 +3133,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -2978,8 +3145,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -2989,8 +3157,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -3000,8 +3169,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -3011,8 +3181,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -3022,8 +3193,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -3033,8 +3205,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -3044,8 +3217,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -3055,8 +3229,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -3066,8 +3241,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
@@ -3077,8 +3253,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3088,8 +3265,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
@@ -3099,8 +3277,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -3110,8 +3289,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -3121,8 +3301,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -3132,8 +3313,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -3143,8 +3325,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -3154,8 +3337,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -3165,8 +3349,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -3176,8 +3361,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="10"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -3187,8 +3373,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -3198,8 +3385,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -3209,8 +3397,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -3220,8 +3409,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -3231,8 +3421,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -3242,8 +3433,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="10"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -3253,8 +3445,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="10"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -3264,8 +3457,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="10"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -3275,8 +3469,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="10"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -3286,8 +3481,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="10"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -3297,8 +3493,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="10"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -3308,8 +3505,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="10"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -3319,8 +3517,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="10"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -3330,8 +3529,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="10"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -3341,8 +3541,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -3352,8 +3553,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="10"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -3363,8 +3565,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="10"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -3374,8 +3577,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="10"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -3385,8 +3589,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="10"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -3396,8 +3601,9 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="10"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -3407,8 +3613,9 @@
         <f t="shared" ref="F73:F106" si="2">IF(A73="","","    { " &amp; $A$1 &amp; ": """ &amp; A73 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B73 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C73) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D73 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E73 &amp; """}" &amp; IF(A74="","",","))</f>
         <v/>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="10"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -3418,8 +3625,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="10"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -3429,8 +3637,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="10"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -3440,8 +3649,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="10"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -3451,8 +3661,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="10"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -3462,8 +3673,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="10"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -3473,8 +3685,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="10"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -3484,8 +3697,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="10"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -3495,8 +3709,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="10"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -3506,8 +3721,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="10"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -3517,8 +3733,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="10"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -3528,8 +3745,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="10"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -3539,8 +3757,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="10"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -3550,8 +3769,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="10"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -3561,8 +3781,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="10"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -3572,8 +3793,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="10"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -3583,8 +3805,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="10"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -3594,8 +3817,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="10"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -3605,8 +3829,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" s="10"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -3616,8 +3841,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="10"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -3627,8 +3853,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="10"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -3638,8 +3865,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="10"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -3649,8 +3877,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="10"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -3660,8 +3889,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="10"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -3671,8 +3901,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97" s="10"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -3682,8 +3913,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98" s="10"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -3693,8 +3925,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99" s="10"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -3704,8 +3937,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100" s="10"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -3715,8 +3949,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G101" s="10"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -3726,8 +3961,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102" s="10"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -3737,8 +3973,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G103" s="10"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -3748,8 +3985,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104" s="10"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="9"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -3759,8 +3997,9 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105" s="10"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="9"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
@@ -3770,6 +4009,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="G106" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3779,21 +4019,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D934C6D7-8A74-4B09-A541-AF970631420F}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F2:F16"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F2:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="125" style="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -3820,131 +4060,135 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
+        <v>233</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>235</v>
+      </c>
       <c r="D2" s="9" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E2" s="9"/>
-      <c r="F2" s="10" t="str">
+      <c r="F2" s="14" t="str">
         <f>IF(A2="","","    { "&amp;$A$1&amp;": """&amp;A2&amp;""", "&amp;$B$1&amp;": """&amp;B2&amp;""", "&amp;$C$1&amp;": """&amp;C2&amp;""", "&amp;$D$1&amp;": """&amp;D2&amp;""", "&amp;$E$1&amp;": """&amp;E2&amp;"""}"&amp;IF(A3="","",","))</f>
-        <v xml:space="preserve">    { id: "home", group: "", name: "", url: "~/default.html", target: ""},</v>
+        <v xml:space="preserve">    { id: "installation_install", group: "Installation", name: "1. Install RasPBX", url: "~/installation/installation.html", target: ""},</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>229</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E3" s="9"/>
-      <c r="F3" s="10" t="str">
-        <f t="shared" ref="F3:F66" si="0">IF(A3="","","    { "&amp;$A$1&amp;": """&amp;A3&amp;""", "&amp;$B$1&amp;": """&amp;B3&amp;""", "&amp;$C$1&amp;": """&amp;C3&amp;""", "&amp;$D$1&amp;": """&amp;D3&amp;""", "&amp;$E$1&amp;": """&amp;E3&amp;"""}"&amp;IF(A4="","",","))</f>
-        <v xml:space="preserve">    { id: "installation_install", group: "Installation", name: "1. Install RasPBX", url: "~/installation/installation.html", target: ""},</v>
+      <c r="F3" s="14" t="str">
+        <f t="shared" ref="F3:F67" si="0">IF(A3="","","    { "&amp;$A$1&amp;": """&amp;A3&amp;""", "&amp;$B$1&amp;": """&amp;B3&amp;""", "&amp;$C$1&amp;": """&amp;C3&amp;""", "&amp;$D$1&amp;": """&amp;D3&amp;""", "&amp;$E$1&amp;": """&amp;E3&amp;"""}"&amp;IF(A4="","",","))</f>
+        <v xml:space="preserve">    { id: "installation_update", group: "Installation", name: "2. Update RasPBX", url: "~/installation/update.html", target: ""},</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>229</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E4" s="9"/>
-      <c r="F4" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "installation_update", group: "Installation", name: "2. Update RasPBX", url: "~/installation/update.html", target: ""},</v>
+      <c r="F4" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "installation_afterupdate", group: "Installation", name: "3. Tasks after update", url: "~/installation/afterupdate.html", target: ""},</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>229</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>268</v>
+        <v>238</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E5" s="9"/>
-      <c r="F5" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "installation_afterupdate", group: "Installation", name: "3. Tasks after update", url: "~/installation/afterupdate.html", target: ""},</v>
+      <c r="F5" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "installation_initialconfig", group: "Installation", name: "4. Initial Configuration", url: "~/installation/initalconfig.html", target: ""},</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "installation_initialconfig", group: "Installation", name: "4. Initial Configuration", url: "~/installation/initalconfig.html", target: ""},</v>
+      <c r="F6" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "remote_terminal", group: "Remote", name: "SSH Terminal", url: "~/remote/terminal.html", target: ""},</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>244</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>245</v>
+        <v>266</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "remote_terminal", group: "Remote", name: "SSH Terminal", url: "~/remote/terminal.html", target: ""},</v>
+      <c r="F7" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "remote_filetransfer", group: "Remote", name: "SSH File Transfer", url: "~/remote/filetransfer.html", target: ""},</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>242</v>
+        <v>309</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>244</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>267</v>
+        <v>310</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "remote_filetransfer", group: "Remote", name: "SSH File Transfer", url: "~/remote/filetransfer.html", target: ""},</v>
+      <c r="F8" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "remote_mariadb", group: "Remote", name: "MariaDB", url: "~/remote/mariadb.html", target: ""},</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3961,186 +4205,212 @@
         <v>252</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="10" t="str">
+      <c r="F9" s="14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">    { id: "phones_linphone", group: "Phones", name: "Linphone (Softphone)", url: "~/phones/linphone.html", target: ""},</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>248</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>271</v>
-      </c>
       <c r="E10" s="9"/>
-      <c r="F10" s="10" t="str">
+      <c r="F10" s="14" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">    { id: "phones_pots", group: "Phones", name: "POTS Connection", url: "~/phones/pots.html", target: ""},</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>248</v>
+        <v>302</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>259</v>
+        <v>304</v>
       </c>
       <c r="E11" s="9"/>
-      <c r="F11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "phones_cisco79xx_reset", group: "Phones", name: "Reset", url: "~/phones/cisco79xx.html", target: ""},</v>
+      <c r="F11" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_tftp", group: "Cisco79xx", name: "Setup TFTP", url: "~/phones/cisco79xx_tftp.html", target: ""},</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>248</v>
+        <v>302</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>259</v>
+        <v>305</v>
       </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "phones_cisco79xx_tftp", group: "Phones", name: "Setup TFTP", url: "~/phones/cisco79xx.html", target: ""},</v>
+      <c r="F12" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_xml", group: "Cisco79xx", name: "XML Config", url: "~/phones/cisco79xx_xml.html", target: ""},</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>248</v>
+        <v>302</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>259</v>
+        <v>303</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "phones_cisco79xx_xml", group: "Phones", name: "XML Config", url: "~/phones/cisco79xx.html", target: ""},</v>
+      <c r="F13" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_reset", group: "Cisco79xx", name: "Reset", url: "~/phones/cisco79xx_reset.html", target: ""},</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>288</v>
+        <v>321</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>248</v>
+        <v>302</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>289</v>
+        <v>323</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>259</v>
+        <v>322</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "phones_cisco79xx_directory", group: "Phones", name: "Directory", url: "~/phones/cisco79xx.html", target: ""},</v>
+      <c r="F14" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_extension", group: "Cisco79xx", name: "Add Extension(s)", url: "~/phones/cisco79xx_extension.html", target: ""},</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>248</v>
+        <v>302</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>259</v>
+        <v>306</v>
       </c>
       <c r="E15" s="9"/>
-      <c r="F15" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "phones_cisco79xx_services", group: "Phones", name: "Services", url: "~/phones/cisco79xx.html", target: ""},</v>
+      <c r="F15" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_directory", group: "Cisco79xx", name: "Directory", url: "~/phones/cisco79xx_directory.html", target: ""},</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx_services", group: "Cisco79xx", name: "Services", url: "~/phones/cisco79xx_services.html", target: ""},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "more_cisco79xx_misc", group: "More", name: "Cisco 79xx Misc. Info", url: "~/more/cisco79xx_misc.html", target: ""},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C18" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "about_references", group: "About", name: "References", url: "~/about/references.html", target: ""}</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="F18" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "about_references", group: "About", name: "References", url: "~/about/references.html", target: ""},</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="D19" s="9" t="s">
+        <v>230</v>
+      </c>
       <c r="E19" s="9"/>
-      <c r="F19" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="F19" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "home", group: "", name: "", url: "~/default.html", target: ""},</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>308</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="F20" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx", group: "Phones", name: "Cisco 79xx", url: "", target: ""}</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4149,7 +4419,7 @@
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="10" t="str">
+      <c r="F21" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4160,7 +4430,7 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="10" t="str">
+      <c r="F22" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4171,7 +4441,7 @@
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="10" t="str">
+      <c r="F23" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4182,7 +4452,7 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="10" t="str">
+      <c r="F24" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4193,7 +4463,7 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="10" t="str">
+      <c r="F25" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4204,7 +4474,7 @@
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="10" t="str">
+      <c r="F26" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4215,7 +4485,7 @@
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="10" t="str">
+      <c r="F27" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4226,7 +4496,7 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="10" t="str">
+      <c r="F28" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4237,7 +4507,7 @@
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="10" t="str">
+      <c r="F29" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4246,9 +4516,9 @@
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="11"/>
+      <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-      <c r="F30" s="10" t="str">
+      <c r="F30" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4257,9 +4527,9 @@
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="9"/>
-      <c r="F31" s="10" t="str">
+      <c r="F31" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4270,7 +4540,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
-      <c r="F32" s="10" t="str">
+      <c r="F32" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4281,7 +4551,7 @@
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
-      <c r="F33" s="10" t="str">
+      <c r="F33" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4292,7 +4562,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
-      <c r="F34" s="10" t="str">
+      <c r="F34" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4303,7 +4573,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
-      <c r="F35" s="10" t="str">
+      <c r="F35" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4314,7 +4584,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
-      <c r="F36" s="10" t="str">
+      <c r="F36" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4325,7 +4595,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
-      <c r="F37" s="10" t="str">
+      <c r="F37" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4336,7 +4606,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
-      <c r="F38" s="10" t="str">
+      <c r="F38" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4347,7 +4617,7 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
-      <c r="F39" s="10" t="str">
+      <c r="F39" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4358,7 +4628,7 @@
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
-      <c r="F40" s="10" t="str">
+      <c r="F40" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4369,7 +4639,7 @@
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
-      <c r="F41" s="10" t="str">
+      <c r="F41" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4380,7 +4650,7 @@
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
-      <c r="F42" s="10" t="str">
+      <c r="F42" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4391,7 +4661,7 @@
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
-      <c r="F43" s="10" t="str">
+      <c r="F43" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4402,7 +4672,7 @@
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
-      <c r="F44" s="10" t="str">
+      <c r="F44" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4413,7 +4683,7 @@
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="9"/>
-      <c r="F45" s="10" t="str">
+      <c r="F45" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4424,7 +4694,7 @@
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
-      <c r="F46" s="10" t="str">
+      <c r="F46" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4435,7 +4705,7 @@
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
-      <c r="F47" s="10" t="str">
+      <c r="F47" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4446,7 +4716,7 @@
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
-      <c r="F48" s="10" t="str">
+      <c r="F48" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4457,7 +4727,7 @@
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
-      <c r="F49" s="10" t="str">
+      <c r="F49" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4468,7 +4738,7 @@
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
-      <c r="F50" s="10" t="str">
+      <c r="F50" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4479,7 +4749,7 @@
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
-      <c r="F51" s="10" t="str">
+      <c r="F51" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4490,7 +4760,7 @@
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
-      <c r="F52" s="10" t="str">
+      <c r="F52" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4501,7 +4771,7 @@
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
-      <c r="F53" s="10" t="str">
+      <c r="F53" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4512,7 +4782,7 @@
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
-      <c r="F54" s="10" t="str">
+      <c r="F54" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4523,7 +4793,7 @@
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
-      <c r="F55" s="10" t="str">
+      <c r="F55" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4534,7 +4804,7 @@
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
-      <c r="F56" s="10" t="str">
+      <c r="F56" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4545,7 +4815,7 @@
       <c r="C57" s="9"/>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
-      <c r="F57" s="10" t="str">
+      <c r="F57" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4556,7 +4826,7 @@
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="E58" s="9"/>
-      <c r="F58" s="10" t="str">
+      <c r="F58" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4567,7 +4837,7 @@
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
-      <c r="F59" s="10" t="str">
+      <c r="F59" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4578,7 +4848,7 @@
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
-      <c r="F60" s="10" t="str">
+      <c r="F60" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4589,7 +4859,7 @@
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
-      <c r="F61" s="10" t="str">
+      <c r="F61" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4600,7 +4870,7 @@
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
-      <c r="F62" s="10" t="str">
+      <c r="F62" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4611,7 +4881,7 @@
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
-      <c r="F63" s="10" t="str">
+      <c r="F63" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4622,7 +4892,7 @@
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
-      <c r="F64" s="10" t="str">
+      <c r="F64" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4633,7 +4903,7 @@
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
       <c r="E65" s="9"/>
-      <c r="F65" s="10" t="str">
+      <c r="F65" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4644,7 +4914,7 @@
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="9"/>
-      <c r="F66" s="10" t="str">
+      <c r="F66" s="14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
@@ -4655,8 +4925,8 @@
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
-      <c r="F67" s="10" t="str">
-        <f t="shared" ref="F67:F106" si="1">IF(A67="","","    { "&amp;$A$1&amp;": """&amp;A67&amp;""", "&amp;$B$1&amp;": """&amp;B67&amp;""", "&amp;$C$1&amp;": """&amp;C67&amp;""", "&amp;$D$1&amp;": """&amp;D67&amp;""", "&amp;$E$1&amp;": """&amp;E67&amp;"""}"&amp;IF(A68="","",","))</f>
+      <c r="F67" s="14" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4666,8 +4936,8 @@
       <c r="C68" s="9"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
-      <c r="F68" s="10" t="str">
-        <f t="shared" si="1"/>
+      <c r="F68" s="14" t="str">
+        <f t="shared" ref="F68:F107" si="1">IF(A68="","","    { "&amp;$A$1&amp;": """&amp;A68&amp;""", "&amp;$B$1&amp;": """&amp;B68&amp;""", "&amp;$C$1&amp;": """&amp;C68&amp;""", "&amp;$D$1&amp;": """&amp;D68&amp;""", "&amp;$E$1&amp;": """&amp;E68&amp;"""}"&amp;IF(A69="","",","))</f>
         <v/>
       </c>
     </row>
@@ -4677,7 +4947,7 @@
       <c r="C69" s="9"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
-      <c r="F69" s="10" t="str">
+      <c r="F69" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4688,7 +4958,7 @@
       <c r="C70" s="9"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
-      <c r="F70" s="10" t="str">
+      <c r="F70" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4699,7 +4969,7 @@
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
-      <c r="F71" s="10" t="str">
+      <c r="F71" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4710,7 +4980,7 @@
       <c r="C72" s="9"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
-      <c r="F72" s="10" t="str">
+      <c r="F72" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4721,7 +4991,7 @@
       <c r="C73" s="9"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
-      <c r="F73" s="10" t="str">
+      <c r="F73" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4732,7 +5002,7 @@
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
-      <c r="F74" s="10" t="str">
+      <c r="F74" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4743,7 +5013,7 @@
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
-      <c r="F75" s="10" t="str">
+      <c r="F75" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4754,7 +5024,7 @@
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="9"/>
-      <c r="F76" s="10" t="str">
+      <c r="F76" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4765,7 +5035,7 @@
       <c r="C77" s="9"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
-      <c r="F77" s="10" t="str">
+      <c r="F77" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4776,7 +5046,7 @@
       <c r="C78" s="9"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
-      <c r="F78" s="10" t="str">
+      <c r="F78" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4787,7 +5057,7 @@
       <c r="C79" s="9"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
-      <c r="F79" s="10" t="str">
+      <c r="F79" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4798,7 +5068,7 @@
       <c r="C80" s="9"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
-      <c r="F80" s="10" t="str">
+      <c r="F80" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4809,7 +5079,7 @@
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
-      <c r="F81" s="10" t="str">
+      <c r="F81" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4820,7 +5090,7 @@
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
-      <c r="F82" s="10" t="str">
+      <c r="F82" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4831,7 +5101,7 @@
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
-      <c r="F83" s="10" t="str">
+      <c r="F83" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4842,7 +5112,7 @@
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
-      <c r="F84" s="10" t="str">
+      <c r="F84" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4853,7 +5123,7 @@
       <c r="C85" s="9"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
-      <c r="F85" s="10" t="str">
+      <c r="F85" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4864,7 +5134,7 @@
       <c r="C86" s="9"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
-      <c r="F86" s="10" t="str">
+      <c r="F86" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4875,7 +5145,7 @@
       <c r="C87" s="9"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
-      <c r="F87" s="10" t="str">
+      <c r="F87" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4886,7 +5156,7 @@
       <c r="C88" s="9"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
-      <c r="F88" s="10" t="str">
+      <c r="F88" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4897,7 +5167,7 @@
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
-      <c r="F89" s="10" t="str">
+      <c r="F89" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4908,7 +5178,7 @@
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
-      <c r="F90" s="10" t="str">
+      <c r="F90" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4919,7 +5189,7 @@
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
-      <c r="F91" s="10" t="str">
+      <c r="F91" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4930,7 +5200,7 @@
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
-      <c r="F92" s="10" t="str">
+      <c r="F92" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4941,7 +5211,7 @@
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
-      <c r="F93" s="10" t="str">
+      <c r="F93" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4952,7 +5222,7 @@
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
-      <c r="F94" s="10" t="str">
+      <c r="F94" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4963,7 +5233,7 @@
       <c r="C95" s="9"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
-      <c r="F95" s="10" t="str">
+      <c r="F95" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4974,7 +5244,7 @@
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
-      <c r="F96" s="10" t="str">
+      <c r="F96" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4985,7 +5255,7 @@
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
-      <c r="F97" s="10" t="str">
+      <c r="F97" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -4996,7 +5266,7 @@
       <c r="C98" s="9"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
-      <c r="F98" s="10" t="str">
+      <c r="F98" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5007,7 +5277,7 @@
       <c r="C99" s="9"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
-      <c r="F99" s="10" t="str">
+      <c r="F99" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5018,7 +5288,7 @@
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
-      <c r="F100" s="10" t="str">
+      <c r="F100" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5029,7 +5299,7 @@
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
-      <c r="F101" s="10" t="str">
+      <c r="F101" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5040,7 +5310,7 @@
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
-      <c r="F102" s="10" t="str">
+      <c r="F102" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5051,7 +5321,7 @@
       <c r="C103" s="9"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
-      <c r="F103" s="10" t="str">
+      <c r="F103" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5062,7 +5332,7 @@
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
-      <c r="F104" s="10" t="str">
+      <c r="F104" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5073,7 +5343,7 @@
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
-      <c r="F105" s="10" t="str">
+      <c r="F105" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5084,7 +5354,18 @@
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
-      <c r="F106" s="10" t="str">
+      <c r="F106" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5103,15 +5384,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="80.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5140,18 +5421,18 @@
         <v>255</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="D2" s="9" t="str">
+        <v>259</v>
+      </c>
+      <c r="D2" s="13" t="str">
         <f>IF(B2="","",B2) &amp; IF(C2="","",C2 &amp; "/")</f>
         <v>installation/installation/</v>
       </c>
-      <c r="E2" s="10" t="str">
+      <c r="E2" s="14" t="str">
         <f>IF(A2="","","    { "&amp;$A$1&amp;": """&amp;A2&amp;""", "&amp;$B$1&amp;": """&amp;B2&amp;""", "&amp;$C$1&amp;": """&amp;C2&amp;""", "&amp;$D$1&amp;": """&amp;D2&amp;"""}"&amp;IF(A3="","",","))</f>
         <v xml:space="preserve">    { name: "installation_install", path: "installation/", file: "installation", resourcePath: "installation/installation/"},</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>234</v>
       </c>
@@ -5159,18 +5440,18 @@
         <v>255</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="D3" s="9" t="str">
-        <f t="shared" ref="D3:D10" si="0">IF(B3="","",B3) &amp; IF(C3="","",C3 &amp; "/")</f>
+        <v>260</v>
+      </c>
+      <c r="D3" s="13" t="str">
+        <f t="shared" ref="D3:D35" si="0">IF(B3="","",B3) &amp; IF(C3="","",C3 &amp; "/")</f>
         <v>installation/update/</v>
       </c>
-      <c r="E3" s="10" t="str">
+      <c r="E3" s="14" t="str">
         <f t="shared" ref="E3:E35" si="1">IF(A3="","","    { "&amp;$A$1&amp;": """&amp;A3&amp;""", "&amp;$B$1&amp;": """&amp;B3&amp;""", "&amp;$C$1&amp;": """&amp;C3&amp;""", "&amp;$D$1&amp;": """&amp;D3&amp;"""}"&amp;IF(A4="","",","))</f>
         <v xml:space="preserve">    { name: "installation_update", path: "installation/", file: "update", resourcePath: "installation/update/"},</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>240</v>
       </c>
@@ -5178,18 +5459,18 @@
         <v>255</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="D4" s="9" t="str">
+        <v>261</v>
+      </c>
+      <c r="D4" s="13" t="str">
         <f t="shared" si="0"/>
         <v>installation/afterupdate/</v>
       </c>
-      <c r="E4" s="10" t="str">
+      <c r="E4" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "installation_afterupdate", path: "installation/", file: "afterupdate", resourcePath: "installation/afterupdate/"},</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>241</v>
       </c>
@@ -5197,18 +5478,18 @@
         <v>255</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="D5" s="9" t="str">
+        <v>262</v>
+      </c>
+      <c r="D5" s="13" t="str">
         <f t="shared" si="0"/>
         <v>installation/initalconfig/</v>
       </c>
-      <c r="E5" s="10" t="str">
+      <c r="E5" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "installation_initialconfig", path: "installation/", file: "initalconfig", resourcePath: "installation/initalconfig/"},</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>243</v>
       </c>
@@ -5216,18 +5497,18 @@
         <v>257</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="D6" s="9" t="str">
+        <v>263</v>
+      </c>
+      <c r="D6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>remote/terminal/</v>
       </c>
-      <c r="E6" s="10" t="str">
+      <c r="E6" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "remote_terminal", path: "remote/", file: "terminal", resourcePath: "remote/terminal/"},</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>242</v>
       </c>
@@ -5235,334 +5516,469 @@
         <v>257</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="D7" s="9" t="str">
+        <v>264</v>
+      </c>
+      <c r="D7" s="13" t="str">
         <f t="shared" si="0"/>
         <v>remote/filetransfer/</v>
       </c>
-      <c r="E7" s="10" t="str">
+      <c r="E7" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "remote_filetransfer", path: "remote/", file: "filetransfer", resourcePath: "remote/filetransfer/"},</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>remote/mariadb/</v>
+      </c>
+      <c r="E8" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "remote_mariadb", path: "remote/", file: "mariadb", resourcePath: "remote/mariadb/"},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>250</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="D8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>phones/linphone/</v>
-      </c>
-      <c r="E8" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "phones_linphone", path: "phones/", file: "linphone", resourcePath: "phones/linphone/"},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>269</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>258</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="D9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>phones/pots/</v>
-      </c>
-      <c r="E9" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "phones_pots", path: "phones/", file: "pots", resourcePath: "phones/pots/"},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="D9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>phones/linphone/</v>
+      </c>
+      <c r="E9" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_linphone", path: "phones/", file: "linphone", resourcePath: "phones/linphone/"},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>258</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>phones/pots/</v>
+      </c>
+      <c r="E10" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_pots", path: "phones/", file: "pots", resourcePath: "phones/pots/"},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="9" t="str">
+      <c r="D11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>phones/cisco79xx/</v>
       </c>
-      <c r="E10" s="10" t="str">
+      <c r="E11" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_cisco79xx_tftp", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>phones/cisco79xx/</v>
+      </c>
+      <c r="E12" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_cisco79xx_xml", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>phones/cisco79xx/</v>
+      </c>
+      <c r="E13" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_cisco79xx_reset", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>phones/cisco79xx/</v>
+      </c>
+      <c r="E14" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_cisco79xx_extension", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D15" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>phones/cisco79xx/</v>
+      </c>
+      <c r="E15" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_cisco79xx_directory", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>phones/cisco79xx/</v>
+      </c>
+      <c r="E16" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_cisco79xx_services", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>more/cisco79xx_misc/</v>
+      </c>
+      <c r="E17" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "more_cisco79xx_misc", path: "more/", file: "cisco79xx_misc", resourcePath: "more/cisco79xx_misc/"},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="13" t="str">
+        <f t="shared" ref="D18:D24" si="2">IF(B18="","",B18) &amp; IF(C18="","",C18 &amp; "/")</f>
+        <v>phones/cisco79xx/</v>
+      </c>
+      <c r="E18" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "phones_cisco79xx", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="D11" s="9" t="str">
-        <f>IF(B11="","",B11) &amp; IF(C11="","",C11 &amp; "/")</f>
+      <c r="D19" s="13" t="str">
+        <f t="shared" si="2"/>
         <v>about/references/</v>
       </c>
-      <c r="E11" s="10" t="str">
+      <c r="E19" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "about_references", path: "about/", file: "references", resourcePath: "about/references/"},</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="D20" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>js/header/</v>
+      </c>
+      <c r="E20" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "test_header", path: "js/", file: "header", resourcePath: "js/header/"},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D21" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>js/footer/</v>
+      </c>
+      <c r="E21" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "test_footer", path: "js/", file: "footer", resourcePath: "js/footer/"},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="D22" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>js/mdbootstrap_footer/</v>
+      </c>
+      <c r="E22" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "sample_mdbootstrap_footer", path: "js/", file: "mdbootstrap_footer", resourcePath: "js/mdbootstrap_footer/"},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="str">
-        <f>IF(B12="","",B12) &amp; IF(C12="","",C12 &amp; "/")</f>
-        <v/>
-      </c>
-      <c r="E12" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "home", path: "", file: "", resourcePath: ""}</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E23" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "home", path: "", file: "", resourcePath: ""}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E24" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E25" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E26" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E27" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E28" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E29" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E30" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E31" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E32" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E33" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E34" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="10" t="str">
+      <c r="D35" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="E35" s="14" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
- Added more information regarding Cisco 79xx extensions - Added content for Cisco 79xx configuration XML files
</commit_message>
<xml_diff>
--- a/DevTools.xlsx
+++ b/DevTools.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/256c97ba8ed48425/Documents/Projects/PBX/RasPBX_Build/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="454" documentId="13_ncr:1_{1C4A9213-C812-4D7A-B2C0-60F82FA4474B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11F528B0-6F11-4568-B797-34DE7F0F4E41}"/>
+  <xr:revisionPtr revIDLastSave="480" documentId="13_ncr:1_{1C4A9213-C812-4D7A-B2C0-60F82FA4474B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{429397E6-E869-46F6-8C28-4D48D5933B05}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{0A6266C4-26DD-4DE6-B06A-1B7D997BFB8E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="328">
   <si>
     <t>URL to Landing Page</t>
   </si>
@@ -766,9 +766,6 @@
     <t>~/installation/afterupdate.html</t>
   </si>
   <si>
-    <t>4. Initial Configuration</t>
-  </si>
-  <si>
     <t>~/installation/initalconfig.html</t>
   </si>
   <si>
@@ -853,9 +850,6 @@
     <t>SSH File Transfer</t>
   </si>
   <si>
-    <t>3. Tasks after update</t>
-  </si>
-  <si>
     <t>phones_pots</t>
   </si>
   <si>
@@ -1022,6 +1016,24 @@
   </si>
   <si>
     <t>Add Extension(s)</t>
+  </si>
+  <si>
+    <t>4. Tasks after Configuration</t>
+  </si>
+  <si>
+    <t>3. Initial Configuration</t>
+  </si>
+  <si>
+    <t>more_windows_utiltiy</t>
+  </si>
+  <si>
+    <t>windows_utility</t>
+  </si>
+  <si>
+    <t>Windows Utility</t>
+  </si>
+  <si>
+    <t>~/more/windows_utility.html</t>
   </si>
 </sst>
 </file>
@@ -2565,21 +2577,21 @@
         <v>108</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>20</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>26</v>
@@ -2588,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F2" s="10" t="str">
         <f>IF(A2="","","    { " &amp; $A$1 &amp; ": """ &amp; A2 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B2 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C2) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D2 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E2 &amp; """}" &amp; IF(A3="","",","))</f>
@@ -2610,10 +2622,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F3" s="10" t="str">
         <f t="shared" ref="F3:F15" si="0">IF(A3="","","    { " &amp; $A$1 &amp; ": """ &amp; A3 &amp; """, " &amp; $B$1 &amp; ": """ &amp; B3 &amp; """, " &amp; C$1 &amp; ": " &amp; LOWER(C3) &amp; ", " &amp; $D$1 &amp; ": """ &amp; D3 &amp; """, " &amp; $E$1 &amp; ": """ &amp; E3 &amp; """}" &amp; IF(A4="","",","))</f>
@@ -2730,7 +2742,7 @@
         <v xml:space="preserve">    { id: "js_header", fileType: "script", req_jquery: true, local: "~/js/header.js", host: "~/js/header.js"},</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2754,12 +2766,12 @@
         <v xml:space="preserve">    { id: "js_footer", fileType: "script", req_jquery: true, local: "~/js/footer.js", host: "~/js/footer.js"},</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>29</v>
@@ -2935,7 +2947,7 @@
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>26</v>
@@ -2944,10 +2956,10 @@
         <v>1</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F18" s="10" t="str">
         <f t="shared" si="1"/>
@@ -4025,7 +4037,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F2:F20"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4104,48 +4116,48 @@
         <v>229</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>267</v>
+        <v>323</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "installation_afterupdate", group: "Installation", name: "3. Tasks after update", url: "~/installation/afterupdate.html", target: ""},</v>
+        <v xml:space="preserve">    { id: "installation_initialconfig", group: "Installation", name: "3. Initial Configuration", url: "~/installation/initalconfig.html", target: ""},</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>229</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>238</v>
+        <v>322</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "installation_initialconfig", group: "Installation", name: "4. Initial Configuration", url: "~/installation/initalconfig.html", target: ""},</v>
+        <v xml:space="preserve">    { id: "installation_afterupdate", group: "Installation", name: "4. Tasks after Configuration", url: "~/installation/afterupdate.html", target: ""},</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>245</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>246</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="14" t="str">
@@ -4155,16 +4167,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="14" t="str">
@@ -4174,16 +4186,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>311</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="14" t="str">
@@ -4193,16 +4205,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>249</v>
-      </c>
       <c r="D9" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="14" t="str">
@@ -4212,16 +4224,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>268</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>270</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="14" t="str">
@@ -4231,16 +4243,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>302</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>304</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="14" t="str">
@@ -4250,16 +4262,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="14" t="str">
@@ -4269,16 +4281,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>282</v>
-      </c>
       <c r="D13" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="14" t="str">
@@ -4288,16 +4300,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>323</v>
-      </c>
       <c r="D14" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="14" t="str">
@@ -4307,16 +4319,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="14" t="str">
@@ -4326,16 +4338,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="14" t="str">
@@ -4345,16 +4357,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>315</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>317</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="14" t="str">
@@ -4364,64 +4376,72 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>272</v>
+        <v>324</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>74</v>
+        <v>313</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "about_references", group: "About", name: "References", url: "~/about/references.html", target: ""},</v>
+        <v xml:space="preserve">    { id: "more_windows_utiltiy", group: "More", name: "Windows Utility", url: "~/more/windows_utility.html", target: ""},</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+        <v>270</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>273</v>
+      </c>
       <c r="D19" s="9" t="s">
-        <v>230</v>
+        <v>274</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "home", group: "", name: "", url: "~/default.html", target: ""},</v>
+        <v xml:space="preserve">    { id: "about_references", group: "About", name: "References", url: "~/about/references.html", target: ""},</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>308</v>
-      </c>
-      <c r="D20" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9" t="s">
+        <v>230</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    { id: "phones_cisco79xx", group: "Phones", name: "Cisco 79xx", url: "", target: ""}</v>
+        <v xml:space="preserve">    { id: "home", group: "", name: "", url: "~/default.html", target: ""},</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>306</v>
+      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="14" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v xml:space="preserve">    { id: "phones_cisco79xx", group: "Phones", name: "Cisco 79xx", url: "", target: ""}</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -5384,7 +5404,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5404,10 +5424,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>254</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>20</v>
@@ -5418,10 +5438,10 @@
         <v>233</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D2" s="13" t="str">
         <f>IF(B2="","",B2) &amp; IF(C2="","",C2 &amp; "/")</f>
@@ -5437,10 +5457,10 @@
         <v>234</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D3" s="13" t="str">
         <f t="shared" ref="D3:D35" si="0">IF(B3="","",B3) &amp; IF(C3="","",C3 &amp; "/")</f>
@@ -5456,48 +5476,48 @@
         <v>240</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>261</v>
       </c>
       <c r="D4" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>installation/afterupdate/</v>
+        <v>installation/initalconfig/</v>
       </c>
       <c r="E4" s="14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "installation_afterupdate", path: "installation/", file: "afterupdate", resourcePath: "installation/afterupdate/"},</v>
+        <v xml:space="preserve">    { name: "installation_initialconfig", path: "installation/", file: "initalconfig", resourcePath: "installation/initalconfig/"},</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D5" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>installation/initalconfig/</v>
+        <v>installation/afterupdate/</v>
       </c>
       <c r="E5" s="14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "installation_initialconfig", path: "installation/", file: "initalconfig", resourcePath: "installation/initalconfig/"},</v>
+        <v xml:space="preserve">    { name: "installation_afterupdate", path: "installation/", file: "afterupdate", resourcePath: "installation/afterupdate/"},</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D6" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5510,13 +5530,13 @@
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5529,13 +5549,13 @@
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D8" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5548,13 +5568,13 @@
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D9" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5567,13 +5587,13 @@
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D10" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5586,13 +5606,13 @@
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D11" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5605,13 +5625,13 @@
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D12" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5624,13 +5644,13 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D13" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5643,13 +5663,13 @@
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D14" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5662,13 +5682,13 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D15" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5681,13 +5701,13 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D16" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5700,13 +5720,13 @@
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>318</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="D17" s="13" t="str">
         <f t="shared" si="0"/>
@@ -5719,116 +5739,122 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>251</v>
+        <v>324</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>258</v>
+        <v>317</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>256</v>
+        <v>325</v>
       </c>
       <c r="D18" s="13" t="str">
         <f t="shared" ref="D18:D24" si="2">IF(B18="","",B18) &amp; IF(C18="","",C18 &amp; "/")</f>
-        <v>phones/cisco79xx/</v>
+        <v>more/windows_utility/</v>
       </c>
       <c r="E18" s="14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "phones_cisco79xx", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+        <v xml:space="preserve">    { name: "more_windows_utiltiy", path: "more/", file: "windows_utility", resourcePath: "more/windows_utility/"},</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D19" s="13" t="str">
+        <f t="shared" si="2"/>
+        <v>phones/cisco79xx/</v>
+      </c>
+      <c r="E19" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "phones_cisco79xx", path: "phones/", file: "cisco79xx", resourcePath: "phones/cisco79xx/"},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="D19" s="13" t="str">
+      <c r="D20" s="13" t="str">
         <f t="shared" si="2"/>
         <v>about/references/</v>
       </c>
-      <c r="E19" s="14" t="str">
+      <c r="E20" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "about_references", path: "about/", file: "references", resourcePath: "about/references/"},</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="D20" s="13" t="str">
+      <c r="C21" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="D21" s="13" t="str">
         <f t="shared" si="2"/>
         <v>js/header/</v>
       </c>
-      <c r="E20" s="14" t="str">
+      <c r="E21" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "test_header", path: "js/", file: "header", resourcePath: "js/header/"},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>294</v>
-      </c>
-      <c r="D21" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v>js/footer/</v>
-      </c>
-      <c r="E21" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "test_footer", path: "js/", file: "footer", resourcePath: "js/footer/"},</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="B22" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>296</v>
-      </c>
       <c r="D22" s="13" t="str">
         <f t="shared" si="2"/>
+        <v>js/footer/</v>
+      </c>
+      <c r="E22" s="14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">    { name: "test_footer", path: "js/", file: "footer", resourcePath: "js/footer/"},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D23" s="13" t="str">
+        <f t="shared" si="2"/>
         <v>js/mdbootstrap_footer/</v>
       </c>
-      <c r="E22" s="14" t="str">
+      <c r="E23" s="14" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve">    { name: "sample_mdbootstrap_footer", path: "js/", file: "mdbootstrap_footer", resourcePath: "js/mdbootstrap_footer/"},</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="13" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E23" s="14" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">    { name: "home", path: "", file: "", resourcePath: ""}</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="13" t="str">
@@ -5837,10 +5863,10 @@
       </c>
       <c r="E24" s="14" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    { name: "home", path: "", file: "", resourcePath: ""}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -5853,7 +5879,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -5866,7 +5892,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -5879,7 +5905,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -5892,7 +5918,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -5905,7 +5931,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -5918,7 +5944,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -5931,7 +5957,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -5944,7 +5970,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -5957,7 +5983,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -5970,7 +5996,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>

</xml_diff>